<commit_message>
Add current year to copyright statement
</commit_message>
<xml_diff>
--- a/files/input_files/BAT_template.xlsx
+++ b/files/input_files/BAT_template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D5CB87-D4A2-4C65-BF64-1A1DF8074EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3E8C77-7411-45E0-9758-0A1211CE298A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="889" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Data sheet'!$A$2:$M$2</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Data sheet'!$A$1:$M$2</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Data sheet totals'!$A$1:$B$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Introduction!$A$1:$A$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Introduction!$A$1:$A$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Data sheet'!$2:$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -109,24 +109,23 @@
     <t>This baseline assessment tool should be used in conjuction with the full guideline. It can be used to evaluate whether practice is in line with the recommendations in the guideline. It can also help to plan activity to meet the recommendations. Access the full guideline through the link below:</t>
   </si>
   <si>
+    <t>Tools and resources to help put the guidance into practice are available on the NICE website. These include resource impact reports and templates to help you identify the financial impact of implementing this guideline. Access the tools and resources through the link below:</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Partial</t>
+  </si>
+  <si>
+    <t>Year of recommendation</t>
+  </si>
+  <si>
     <t>National Institute for Health and Care Excellence
-Level 1A, City Tower, Piccadilly Plaza, Manchester M1 4BT; www.nice.org.uk
-© NICE 2022. All rights reserved.</t>
-  </si>
-  <si>
-    <t>Tools and resources to help put the guidance into practice are available on the NICE website. These include resource impact reports and templates to help you identify the financial impact of implementing this guideline. Access the tools and resources through the link below:</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Partial</t>
-  </si>
-  <si>
-    <t>Year of recommendation</t>
+Level 1A, City Tower, Piccadilly Plaza, Manchester M1 4BT; www.nice.org.uk</t>
   </si>
 </sst>
 </file>
@@ -570,14 +569,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>298450</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>22225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4077564</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>25390</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>21580</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -944,9 +943,11 @@
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E155"/>
+  <dimension ref="A1:E156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -994,21 +995,21 @@
     </row>
     <row r="9" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
     </row>
-    <row r="11" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-    </row>
-    <row r="13" spans="1:5" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
     </row>
     <row r="14" spans="1:5" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
@@ -1017,12 +1018,14 @@
     <row r="15" spans="1:5" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
     </row>
-    <row r="16" spans="1:5" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:5" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+    </row>
     <row r="17" spans="1:1" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:1" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-    </row>
-    <row r="19" spans="1:1" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:1" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:1" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+    </row>
     <row r="20" spans="1:1" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:1" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:1" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25"/>
@@ -1158,7 +1161,8 @@
     <row r="152" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25"/>
     <row r="153" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25"/>
     <row r="154" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25"/>
-    <row r="155" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="155" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.25"/>
+    <row r="156" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1218,7 +1222,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>14</v>
@@ -1868,17 +1872,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alter template to remove errors in year column
</commit_message>
<xml_diff>
--- a/files/input_files/BAT_template.xlsx
+++ b/files/input_files/BAT_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3E8C77-7411-45E0-9758-0A1211CE298A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED65CE8-C874-49AF-A2C9-E9ABCA0F484B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="889" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,7 +430,7 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -518,6 +518,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -945,9 +948,7 @@
   </sheetPr>
   <dimension ref="A1:E156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1175,7 +1176,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -1254,6 +1255,15 @@
       <c r="M2" s="27" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C3" s="30"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C5" s="30"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C12" s="30"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:M2" xr:uid="{CDAB6358-A15C-45A3-97A4-BA9D51CB315E}"/>

</xml_diff>

<commit_message>
Adjust scrape_docx funtion to allow for additional bullet style
</commit_message>
<xml_diff>
--- a/files/input_files/BAT_template.xlsx
+++ b/files/input_files/BAT_template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED65CE8-C874-49AF-A2C9-E9ABCA0F484B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBF9C40-81F7-4F00-8447-B45BD918CDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="889" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>